<commit_message>
Ajustes de Configuraciones 1
</commit_message>
<xml_diff>
--- a/alimentos.xlsx
+++ b/alimentos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,86 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-08-13 10:27:18</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MILK</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>620.00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>33.30</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>54.20</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>33.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-08-13 10:27:50</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BURGER KING, french fries</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>280.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>38.70</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>